<commit_message>
Done with 183 challenge
</commit_message>
<xml_diff>
--- a/CH-183 Match the Dates.xlsx
+++ b/CH-183 Match the Dates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63B2CD0-B450-4763-909A-9FAD81C87225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3736E9BD-2B33-4E2F-8B36-FEE1EF1EB891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
   <si>
     <t>Result</t>
   </si>
@@ -135,6 +136,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
+  </si>
+  <si>
+    <t>This is a good way</t>
   </si>
 </sst>
 </file>
@@ -381,7 +385,124 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -866,30 +987,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}" name="Data" displayName="Data" ref="C2:C29" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}" name="Data" displayName="Data" ref="C2:C29" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="C2:C29" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E9D2B9E8-BF22-47EC-9F78-4895D7ECD803}" name="Date" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{E9D2B9E8-BF22-47EC-9F78-4895D7ECD803}" name="Date" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{611DC4ED-774C-4CD3-A739-69AFD0B9B007}" name="Data3" displayName="Data3" ref="C2:C29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{611DC4ED-774C-4CD3-A739-69AFD0B9B007}" name="Data3" displayName="Data3" ref="C2:C29" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="C2:C29" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C572AF84-891F-4CB4-8788-F4A5E5A201A3}" name="Date" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{C572AF84-891F-4CB4-8788-F4A5E5A201A3}" name="Date" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F2584124-639F-4080-AE95-344B54195C0B}" name="Data4" displayName="Data4" ref="C2:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F2584124-639F-4080-AE95-344B54195C0B}" name="Data4" displayName="Data4" ref="C2:C29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
   <autoFilter ref="C2:C29" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3295D2D5-3773-4785-9D16-716C0FD5ACEB}" name="Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3295D2D5-3773-4785-9D16-716C0FD5ACEB}" name="Date" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B7C3CE6F-572A-4E9E-87BD-4A8F1B5D23B0}" name="Data5" displayName="Data5" ref="C2:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+  <autoFilter ref="C2:C29" xr:uid="{E4CF8740-D44D-4159-9A33-0E87A0950599}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5A2E3570-8610-4DDC-8114-8DDF881F8F97}" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1161,7 +1292,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="733" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="933" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1467,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A99F12-692D-4B36-B374-084E04C38703}">
   <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2573,7 +2704,7 @@
   <dimension ref="B1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2623,7 +2754,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" cm="1">
+      <c r="E3" s="8" cm="1">
         <f t="array" ref="E3:E19">_xlfn.LET(
     _xlpm.d, C3:C29,
     _xlpm.R, _xleta.REGEXEXTRACT,
@@ -2651,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>45284</v>
       </c>
       <c r="F4" s="4"/>
@@ -2666,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <v>45649</v>
       </c>
       <c r="F5" s="4"/>
@@ -2681,7 +2812,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
         <v>46015</v>
       </c>
       <c r="F6" s="4"/>
@@ -2696,7 +2827,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="4">
+      <c r="E7" s="8">
         <v>46380</v>
       </c>
       <c r="F7" s="4"/>
@@ -2711,7 +2842,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4">
+      <c r="E8" s="8">
         <v>47111</v>
       </c>
       <c r="F8" s="4"/>
@@ -2726,7 +2857,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4">
+      <c r="E9" s="8">
         <v>11316</v>
       </c>
       <c r="F9" s="4"/>
@@ -2741,7 +2872,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4">
+      <c r="E10" s="8">
         <v>45656</v>
       </c>
       <c r="F10" s="4"/>
@@ -2756,7 +2887,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="E11" s="8">
         <v>37281</v>
       </c>
       <c r="F11" s="4"/>
@@ -2770,7 +2901,7 @@
       <c r="C12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="8">
         <v>37646</v>
       </c>
       <c r="I12" s="8">
@@ -2781,7 +2912,7 @@
       <c r="C13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="8">
         <v>45660</v>
       </c>
       <c r="I13" s="8">
@@ -2792,7 +2923,7 @@
       <c r="C14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="8">
         <v>38011</v>
       </c>
       <c r="I14" s="8">
@@ -2803,7 +2934,7 @@
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="8">
         <v>38377</v>
       </c>
     </row>
@@ -2811,7 +2942,7 @@
       <c r="C16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="8">
         <v>38742</v>
       </c>
     </row>
@@ -2819,7 +2950,7 @@
       <c r="C17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="8">
         <v>45663</v>
       </c>
     </row>
@@ -2827,7 +2958,7 @@
       <c r="C18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="8">
         <v>39472</v>
       </c>
     </row>
@@ -2835,7 +2966,7 @@
       <c r="C19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="8">
         <v>45665</v>
       </c>
     </row>
@@ -2885,6 +3016,322 @@
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C279A03-096D-48E7-AA12-89951F6C3F85}">
+  <dimension ref="B1:L29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.8984375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="2.09765625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="8" cm="1">
+        <f t="array" ref="E3:E14">_xlfn.UNIQUE(
+    _xlfn.MAP(
+        Data[Date],
+        _xlfn.LAMBDA(_xlpm.x,
+            _xlfn.LET(
+                _xlpm.a, _xlfn.TEXTSPLIT(_xlpm.x, {"-","/"," "}),
+                _xlpm.b, _xleta.INDEX,
+                DATEVALUE(_xlpm.b(_xlpm.a, , 3) &amp; "/" &amp; _xlpm.b(_xlpm.a, , 2) &amp; "/" &amp; _xlpm.b(_xlpm.a, , 1))
+            )
+        )
+    )
+)</f>
+        <v>45648</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="8">
+        <v>45648</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="8">
+        <v>45649</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="8">
+        <v>45649</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="8">
+        <v>45651</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="8">
+        <v>45651</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="8">
+        <v>45652</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="8">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="8">
+        <v>45654</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="8">
+        <v>45654</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="8">
+        <v>45656</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="8">
+        <v>45656</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="8">
+        <v>45659</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="8">
+        <v>45659</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="8">
+        <v>45660</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="8">
+        <v>45660</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="8">
+        <v>45661</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="8">
+        <v>45661</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8">
+        <v>45662</v>
+      </c>
+      <c r="I12" s="8">
+        <v>45662</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8">
+        <v>45663</v>
+      </c>
+      <c r="I13" s="8">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="8">
+        <v>45665</v>
+      </c>
+      <c r="I14" s="8">
+        <v>45665</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" s="20" t="s">
         <v>22</v>
       </c>

</xml_diff>